<commit_message>
Create frontend and change database 201712140549
</commit_message>
<xml_diff>
--- a/Docs/dictionarydata20171214.xlsx
+++ b/Docs/dictionarydata20171214.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680" xr2:uid="{F073F19D-9989-485C-A11E-104FFE5C4E07}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680" xr2:uid="{60400389-481C-4620-A326-8575E2E6C68F}"/>
   </bookViews>
   <sheets>
     <sheet name="Trang_tính1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="97">
   <si>
     <t>account</t>
   </si>
@@ -155,10 +155,13 @@
     <t>apikey</t>
   </si>
   <si>
-    <t>valueApi</t>
-  </si>
-  <si>
-    <t>char(20)</t>
+    <t>statusApi</t>
+  </si>
+  <si>
+    <t>bit(1)</t>
+  </si>
+  <si>
+    <t>b'1'</t>
   </si>
   <si>
     <t>encriptApi</t>
@@ -330,12 +333,6 @@
   </si>
   <si>
     <t>isStudent</t>
-  </si>
-  <si>
-    <t>bit(1)</t>
-  </si>
-  <si>
-    <t>b'1'</t>
   </si>
   <si>
     <t>staff</t>
@@ -603,7 +600,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" tgtFrame="_blank" tooltip="Open new phpMyAdmin window"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF5CA236-C070-49D7-8AC5-7430DFBB6281}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21CD8F06-0B81-4321-9FA2-FCBBC979202D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -945,11 +942,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D75AA65B-DA51-4CE4-B5EB-5981316E67B7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2492620-9BC2-4E22-B906-D296D02E1520}">
   <dimension ref="A1:I176"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A191" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -958,6 +955,10 @@
     <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1232,17 +1233,19 @@
       <c r="C21" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="4"/>
+      <c r="D21" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
     </row>
     <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>10</v>
@@ -1324,7 +1327,7 @@
     </row>
     <row r="29" spans="1:9" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1358,7 +1361,7 @@
         <v>8</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>10</v>
@@ -1370,24 +1373,24 @@
     </row>
     <row r="33" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>40</v>
       </c>
       <c r="C33" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D33" s="4"/>
       <c r="E33" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
     </row>
     <row r="34" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>14</v>
@@ -1402,10 +1405,10 @@
     </row>
     <row r="35" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>17</v>
@@ -1419,10 +1422,10 @@
     </row>
     <row r="36" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>45</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>17</v>
@@ -1503,7 +1506,7 @@
     </row>
     <row r="42" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>30</v>
@@ -1515,7 +1518,7 @@
         <v>10</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F42" s="6">
         <v>0</v>
@@ -1530,7 +1533,7 @@
     </row>
     <row r="43" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>30</v>
@@ -1542,7 +1545,7 @@
         <v>10</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F43" s="6">
         <v>0</v>
@@ -1560,7 +1563,7 @@
     </row>
     <row r="45" spans="1:9" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1601,17 +1604,17 @@
       </c>
       <c r="D48" s="4"/>
       <c r="E48" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
     </row>
     <row r="49" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C49" s="6" t="s">
         <v>10</v>
@@ -1623,7 +1626,7 @@
     </row>
     <row r="50" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>14</v>
@@ -1710,7 +1713,7 @@
     </row>
     <row r="57" spans="1:9" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1744,7 +1747,7 @@
         <v>8</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C60" s="6" t="s">
         <v>10</v>
@@ -1756,10 +1759,10 @@
     </row>
     <row r="61" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C61" s="6" t="s">
         <v>10</v>
@@ -1771,10 +1774,10 @@
     </row>
     <row r="62" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C62" s="6" t="s">
         <v>10</v>
@@ -1786,10 +1789,10 @@
     </row>
     <row r="63" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B63" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>57</v>
       </c>
       <c r="C63" s="6" t="s">
         <v>10</v>
@@ -1801,10 +1804,10 @@
     </row>
     <row r="64" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C64" s="6" t="s">
         <v>10</v>
@@ -1816,10 +1819,10 @@
     </row>
     <row r="65" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C65" s="6" t="s">
         <v>10</v>
@@ -1831,10 +1834,10 @@
     </row>
     <row r="66" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C66" s="6" t="s">
         <v>17</v>
@@ -1848,7 +1851,7 @@
     </row>
     <row r="67" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B67" s="5" t="s">
         <v>9</v>
@@ -1863,7 +1866,7 @@
     </row>
     <row r="68" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B68" s="5" t="s">
         <v>9</v>
@@ -1948,7 +1951,7 @@
     </row>
     <row r="75" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1994,7 +1997,7 @@
     </row>
     <row r="79" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B79" s="5" t="s">
         <v>14</v>
@@ -2009,10 +2012,10 @@
     </row>
     <row r="80" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C80" s="6" t="s">
         <v>10</v>
@@ -2095,7 +2098,7 @@
       <c r="C86" s="10"/>
       <c r="D86" s="10"/>
       <c r="E86" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F86" s="6">
         <v>0</v>
@@ -2113,7 +2116,7 @@
     </row>
     <row r="88" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2159,7 +2162,7 @@
     </row>
     <row r="92" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B92" s="5" t="s">
         <v>14</v>
@@ -2174,10 +2177,10 @@
     </row>
     <row r="93" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C93" s="6" t="s">
         <v>10</v>
@@ -2189,7 +2192,7 @@
     </row>
     <row r="94" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B94" s="5" t="s">
         <v>14</v>
@@ -2277,7 +2280,7 @@
       <c r="C100" s="10"/>
       <c r="D100" s="10"/>
       <c r="E100" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F100" s="6">
         <v>0</v>
@@ -2292,7 +2295,7 @@
     </row>
     <row r="101" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B101" s="6" t="s">
         <v>30</v>
@@ -2304,7 +2307,7 @@
         <v>10</v>
       </c>
       <c r="E101" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F101" s="6">
         <v>0</v>
@@ -2322,7 +2325,7 @@
     </row>
     <row r="103" spans="1:9" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="104" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2371,7 +2374,7 @@
         <v>19</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C107" s="6" t="s">
         <v>10</v>
@@ -2383,7 +2386,7 @@
     </row>
     <row r="108" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B108" s="5" t="s">
         <v>9</v>
@@ -2400,7 +2403,7 @@
     </row>
     <row r="109" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B109" s="5" t="s">
         <v>12</v>
@@ -2485,7 +2488,7 @@
     </row>
     <row r="116" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="117" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2519,7 +2522,7 @@
         <v>8</v>
       </c>
       <c r="B119" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C119" s="6" t="s">
         <v>10</v>
@@ -2531,7 +2534,7 @@
     </row>
     <row r="120" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B120" s="5" t="s">
         <v>14</v>
@@ -2546,17 +2549,17 @@
     </row>
     <row r="121" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B121" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="B121" s="5" t="s">
-        <v>40</v>
       </c>
       <c r="C121" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D121" s="4"/>
       <c r="E121" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F121" s="6"/>
       <c r="G121" s="6"/>
@@ -2630,7 +2633,7 @@
     </row>
     <row r="127" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B127" s="6" t="s">
         <v>30</v>
@@ -2642,7 +2645,7 @@
         <v>10</v>
       </c>
       <c r="E127" s="6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F127" s="6">
         <v>0</v>
@@ -2660,7 +2663,7 @@
     </row>
     <row r="129" spans="1:9" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="130" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2706,7 +2709,7 @@
     </row>
     <row r="133" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B133" s="5" t="s">
         <v>14</v>
@@ -2716,14 +2719,14 @@
       </c>
       <c r="D133" s="4"/>
       <c r="E133" s="6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F133" s="6"/>
       <c r="G133" s="6"/>
     </row>
     <row r="134" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B134" s="5" t="s">
         <v>14</v>
@@ -2740,16 +2743,16 @@
     </row>
     <row r="135" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B135" s="5" t="s">
-        <v>82</v>
+        <v>36</v>
       </c>
       <c r="C135" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D135" s="4" t="s">
-        <v>83</v>
+        <v>37</v>
       </c>
       <c r="E135" s="6"/>
       <c r="F135" s="6"/>
@@ -2828,7 +2831,7 @@
       <c r="C141" s="10"/>
       <c r="D141" s="10"/>
       <c r="E141" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F141" s="6">
         <v>0</v>
@@ -2843,7 +2846,7 @@
     </row>
     <row r="142" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B142" s="6" t="s">
         <v>30</v>
@@ -2855,7 +2858,7 @@
         <v>10</v>
       </c>
       <c r="E142" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F142" s="6">
         <v>0</v>
@@ -2873,7 +2876,7 @@
     </row>
     <row r="144" spans="1:9" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="145" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2919,7 +2922,7 @@
     </row>
     <row r="148" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B148" s="5" t="s">
         <v>14</v>
@@ -2934,10 +2937,10 @@
     </row>
     <row r="149" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B149" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C149" s="6" t="s">
         <v>10</v>
@@ -2949,10 +2952,10 @@
     </row>
     <row r="150" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B150" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C150" s="6" t="s">
         <v>10</v>
@@ -2964,7 +2967,7 @@
     </row>
     <row r="151" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B151" s="5" t="s">
         <v>9</v>
@@ -3052,7 +3055,7 @@
       <c r="C157" s="10"/>
       <c r="D157" s="10"/>
       <c r="E157" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F157" s="6">
         <v>0</v>
@@ -3067,7 +3070,7 @@
     </row>
     <row r="158" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A158" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B158" s="6" t="s">
         <v>30</v>
@@ -3079,7 +3082,7 @@
         <v>10</v>
       </c>
       <c r="E158" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F158" s="6">
         <v>0</v>
@@ -3097,7 +3100,7 @@
     </row>
     <row r="160" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="161" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3143,7 +3146,7 @@
     </row>
     <row r="164" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B164" s="5" t="s">
         <v>14</v>
@@ -3158,10 +3161,10 @@
     </row>
     <row r="165" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B165" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C165" s="6" t="s">
         <v>10</v>
@@ -3173,10 +3176,10 @@
     </row>
     <row r="166" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B166" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C166" s="6" t="s">
         <v>10</v>
@@ -3188,7 +3191,7 @@
     </row>
     <row r="167" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B167" s="5" t="s">
         <v>14</v>
@@ -3200,7 +3203,7 @@
         <v>18</v>
       </c>
       <c r="E167" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F167" s="6"/>
       <c r="G167" s="6"/>
@@ -3278,7 +3281,7 @@
       <c r="C173" s="10"/>
       <c r="D173" s="10"/>
       <c r="E173" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F173" s="6">
         <v>0</v>
@@ -3293,7 +3296,7 @@
     </row>
     <row r="174" spans="1:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B174" s="6" t="s">
         <v>30</v>
@@ -3305,7 +3308,7 @@
         <v>10</v>
       </c>
       <c r="E174" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F174" s="6">
         <v>0</v>

</xml_diff>